<commit_message>
add service system code
</commit_message>
<xml_diff>
--- a/system/data/wether_conditons_types.xlsx
+++ b/system/data/wether_conditons_types.xlsx
@@ -5,7 +5,7 @@
   <x:workbookPr date1904="0" showBorderUnselectedTables="1" filterPrivacy="0" promptedSolutions="0" showInkAnnotation="1" backupFile="0" saveExternalLinkValues="1" codeName="ThisWorkbook" hidePivotFieldList="0" allowRefreshQuery="0" publishItems="0" checkCompatibility="0" autoCompressPictures="1" refreshAllConnections="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Project\LOCATADS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Project\LOCATADS\system\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <x:bookViews>
@@ -19,153 +19,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
+<x:sst xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <x:si>
-    <x:t>Thundery outbreaks possible</x:t>
+    <x:t>cloudy</x:t>
   </x:si>
   <x:si>
-    <x:t>Fog</x:t>
+    <x:t>snowy</x:t>
   </x:si>
   <x:si>
-    <x:t>Patchy sleet possible</x:t>
+    <x:t>sunny</x:t>
   </x:si>
   <x:si>
-    <x:t>Patchy snow possible</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Patchy light drizzle</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Heavy freezing drizzle</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Moderate rain at times</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Moderate or heavy sleet</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Patchy moderate snow</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Torrential rain shower</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Patchy rain possible</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Sunny</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Cloudy</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mist</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Partly cloudy</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Moderate rain</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Light drizzle</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Blowing snow</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Freezing fog</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Moderate snow</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Moderate or heavy showers of ice pellets</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Moderate or heavy freezing rain</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Patchy light rain with thunder</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Moderate or heavy rain shower</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Light showers of ice pellets</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Moderate or heavy sleet showers</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Light rain shower</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Patchy light snow</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Patchy light rain</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Patchy heavy snow</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Light freezing rain</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Light sleet showers</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Freezing drizzle</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Heavy rain at times</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Overcast</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Blizzard</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Light rain</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Heavy rain</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Light snow</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Light sleet</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Ice pellets</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Heavy snow</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Patchy light snow with thunder</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Moderate or heavy snow with thunder</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Moderate or heavy rain with thunder</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Patchy freezing drizzle possible</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Rainy</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Snowy</x:t>
-  </x:si>
-  <x:si>
-    <x:t>types</x:t>
+    <x:t>rainy</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -233,7 +98,10 @@
       <x:alignment horizontal="general" vertical="center"/>
     </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="1">
+  <x:cellXfs count="2">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <x:alignment horizontal="general" vertical="center"/>
+    </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <x:alignment horizontal="general" vertical="center"/>
     </x:xf>
@@ -891,371 +759,216 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheetPr codeName="Sheet1"/>
-  <x:dimension ref="A2:I21"/>
+  <x:dimension ref="A2:D21"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" topLeftCell="A1" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <x:selection activeCell="F26" activeCellId="0" sqref="F26:F26"/>
+      <x:selection activeCell="G6" activeCellId="0" sqref="G6:G6"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="16.399999999999999"/>
   <x:cols>
-    <x:col min="3" max="3" width="9.00390625" customWidth="1"/>
-    <x:col min="5" max="5" width="9.00390625" customWidth="1"/>
-    <x:col min="6" max="6" width="13.03125" bestFit="1" customWidth="1"/>
-    <x:col min="7" max="7" width="13.03125" customWidth="1"/>
+    <x:col min="1" max="2" width="9.00390625" style="1" customWidth="1"/>
+    <x:col min="3" max="3" width="13.03125" style="1" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="2" spans="1:8">
-      <x:c r="A2" t="s">
-        <x:v>48</x:v>
-      </x:c>
-      <x:c r="B2" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="C2">
+    <x:row r="2" spans="1:4">
+      <x:c r="A2" s="1" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="B2" s="1" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="C2" s="1" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="D2" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:4">
+      <x:c r="A3" s="1">
         <x:v>1000</x:v>
       </x:c>
-      <x:c r="D2" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="E2">
+      <x:c r="B3" s="1">
+        <x:v>1003</x:v>
+      </x:c>
+      <x:c r="C3" s="1">
+        <x:v>1114</x:v>
+      </x:c>
+      <x:c r="D3" s="1">
+        <x:v>1150</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="2:4">
+      <x:c r="B4" s="1">
         <x:v>1006</x:v>
       </x:c>
-      <x:c r="F2" t="s">
-        <x:v>47</x:v>
-      </x:c>
-      <x:c r="H2" t="s">
-        <x:v>46</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="3" spans="2:9">
-      <x:c r="B3" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="C3">
-        <x:v>1000</x:v>
-      </x:c>
-      <x:c r="D3" t="s">
-        <x:v>14</x:v>
-      </x:c>
-      <x:c r="E3">
-        <x:v>1003</x:v>
-      </x:c>
-      <x:c r="F3" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="G3">
-        <x:v>1114</x:v>
-      </x:c>
-      <x:c r="H3" t="s">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="I3">
-        <x:v>1150</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="4" spans="4:9">
-      <x:c r="D4" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="E4">
-        <x:v>1006</x:v>
-      </x:c>
-      <x:c r="F4" t="s">
-        <x:v>35</x:v>
-      </x:c>
-      <x:c r="G4">
+      <x:c r="C4" s="1">
         <x:v>1117</x:v>
       </x:c>
-      <x:c r="H4" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="I4">
+      <x:c r="D4" s="1">
         <x:v>1153</x:v>
       </x:c>
     </x:row>
-    <x:row r="5" spans="4:9">
-      <x:c r="D5" t="s">
-        <x:v>34</x:v>
-      </x:c>
-      <x:c r="E5">
+    <x:row r="5" spans="2:4">
+      <x:c r="B5" s="1">
         <x:v>1009</x:v>
       </x:c>
-      <x:c r="F5" t="s">
-        <x:v>39</x:v>
-      </x:c>
-      <x:c r="G5">
+      <x:c r="C5" s="1">
         <x:v>1204</x:v>
       </x:c>
-      <x:c r="H5" t="s">
-        <x:v>32</x:v>
-      </x:c>
-      <x:c r="I5">
+      <x:c r="D5" s="1">
         <x:v>1168</x:v>
       </x:c>
     </x:row>
-    <x:row r="6" spans="4:9">
-      <x:c r="D6" t="s">
-        <x:v>13</x:v>
-      </x:c>
-      <x:c r="E6">
+    <x:row r="6" spans="2:4">
+      <x:c r="B6" s="1">
         <x:v>1030</x:v>
       </x:c>
-      <x:c r="F6" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="G6">
+      <x:c r="C6" s="1">
         <x:v>1207</x:v>
       </x:c>
-      <x:c r="H6" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="I6">
+      <x:c r="D6" s="1">
         <x:v>1171</x:v>
       </x:c>
     </x:row>
-    <x:row r="7" spans="4:9">
-      <x:c r="D7" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="E7">
+    <x:row r="7" spans="2:4">
+      <x:c r="B7" s="1">
         <x:v>1063</x:v>
       </x:c>
-      <x:c r="F7" t="s">
-        <x:v>27</x:v>
-      </x:c>
-      <x:c r="G7">
+      <x:c r="C7" s="1">
         <x:v>1210</x:v>
       </x:c>
-      <x:c r="H7" t="s">
-        <x:v>28</x:v>
-      </x:c>
-      <x:c r="I7">
+      <x:c r="D7" s="1">
         <x:v>1180</x:v>
       </x:c>
     </x:row>
-    <x:row r="8" spans="4:9">
-      <x:c r="D8" t="s">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="E8">
+    <x:row r="8" spans="2:4">
+      <x:c r="B8" s="1">
         <x:v>1066</x:v>
       </x:c>
-      <x:c r="F8" t="s">
-        <x:v>38</x:v>
-      </x:c>
-      <x:c r="G8">
+      <x:c r="C8" s="1">
         <x:v>1213</x:v>
       </x:c>
-      <x:c r="H8" t="s">
-        <x:v>36</x:v>
-      </x:c>
-      <x:c r="I8">
+      <x:c r="D8" s="1">
         <x:v>1183</x:v>
       </x:c>
     </x:row>
-    <x:row r="9" spans="4:9">
-      <x:c r="D9" t="s">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="E9">
+    <x:row r="9" spans="2:4">
+      <x:c r="B9" s="1">
         <x:v>1069</x:v>
       </x:c>
-      <x:c r="F9" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="G9">
+      <x:c r="C9" s="1">
         <x:v>1216</x:v>
       </x:c>
-      <x:c r="H9" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="I9">
+      <x:c r="D9" s="1">
         <x:v>1186</x:v>
       </x:c>
     </x:row>
-    <x:row r="10" spans="4:9">
-      <x:c r="D10" t="s">
-        <x:v>45</x:v>
-      </x:c>
-      <x:c r="E10">
+    <x:row r="10" spans="2:4">
+      <x:c r="B10" s="1">
         <x:v>1072</x:v>
       </x:c>
-      <x:c r="F10" t="s">
-        <x:v>19</x:v>
-      </x:c>
-      <x:c r="G10">
+      <x:c r="C10" s="1">
         <x:v>1219</x:v>
       </x:c>
-      <x:c r="H10" t="s">
-        <x:v>15</x:v>
-      </x:c>
-      <x:c r="I10">
+      <x:c r="D10" s="1">
         <x:v>1189</x:v>
       </x:c>
     </x:row>
-    <x:row r="11" spans="4:9">
-      <x:c r="D11" t="s">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="E11">
+    <x:row r="11" spans="2:4">
+      <x:c r="B11" s="1">
         <x:v>1087</x:v>
       </x:c>
-      <x:c r="F11" t="s">
-        <x:v>29</x:v>
-      </x:c>
-      <x:c r="G11">
+      <x:c r="C11" s="1">
         <x:v>1222</x:v>
       </x:c>
-      <x:c r="H11" t="s">
-        <x:v>33</x:v>
-      </x:c>
-      <x:c r="I11">
+      <x:c r="D11" s="1">
         <x:v>1192</x:v>
       </x:c>
     </x:row>
-    <x:row r="12" spans="4:9">
-      <x:c r="D12" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="E12">
+    <x:row r="12" spans="2:4">
+      <x:c r="B12" s="1">
         <x:v>1135</x:v>
       </x:c>
-      <x:c r="F12" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="G12">
+      <x:c r="C12" s="1">
         <x:v>1225</x:v>
       </x:c>
-      <x:c r="H12" t="s">
-        <x:v>37</x:v>
-      </x:c>
-      <x:c r="I12">
+      <x:c r="D12" s="1">
         <x:v>1195</x:v>
       </x:c>
     </x:row>
-    <x:row r="13" spans="4:9">
-      <x:c r="D13" t="s">
-        <x:v>18</x:v>
-      </x:c>
-      <x:c r="E13">
+    <x:row r="13" spans="2:4">
+      <x:c r="B13" s="1">
         <x:v>1147</x:v>
       </x:c>
-      <x:c r="F13" t="s">
-        <x:v>40</x:v>
-      </x:c>
-      <x:c r="G13">
+      <x:c r="C13" s="1">
         <x:v>1237</x:v>
       </x:c>
-      <x:c r="H13" t="s">
-        <x:v>30</x:v>
-      </x:c>
-      <x:c r="I13">
+      <x:c r="D13" s="1">
         <x:v>1198</x:v>
       </x:c>
     </x:row>
-    <x:row r="14" spans="6:9">
-      <x:c r="F14" t="s">
-        <x:v>24</x:v>
-      </x:c>
-      <x:c r="G14">
+    <x:row r="14" spans="3:4">
+      <x:c r="C14" s="1">
         <x:v>1261</x:v>
       </x:c>
-      <x:c r="H14" t="s">
-        <x:v>21</x:v>
-      </x:c>
-      <x:c r="I14">
+      <x:c r="D14" s="1">
         <x:v>1201</x:v>
       </x:c>
     </x:row>
-    <x:row r="15" spans="6:9">
-      <x:c r="F15" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="G15">
+    <x:row r="15" spans="3:4">
+      <x:c r="C15" s="1">
         <x:v>1264</x:v>
       </x:c>
-      <x:c r="H15" t="s">
-        <x:v>26</x:v>
-      </x:c>
-      <x:c r="I15">
+      <x:c r="D15" s="1">
         <x:v>1240</x:v>
       </x:c>
     </x:row>
-    <x:row r="16" spans="6:9">
-      <x:c r="F16" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="G16">
+    <x:row r="16" spans="3:4">
+      <x:c r="C16" s="1">
         <x:v>1273</x:v>
       </x:c>
-      <x:c r="H16" t="s">
-        <x:v>23</x:v>
-      </x:c>
-      <x:c r="I16">
+      <x:c r="D16" s="1">
         <x:v>1243</x:v>
       </x:c>
     </x:row>
-    <x:row r="17" spans="6:9">
-      <x:c r="F17" t="s">
-        <x:v>44</x:v>
-      </x:c>
-      <x:c r="G17">
+    <x:row r="17" spans="3:4">
+      <x:c r="C17" s="1">
         <x:v>1276</x:v>
       </x:c>
-      <x:c r="H17" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="I17">
+      <x:c r="D17" s="1">
         <x:v>1246</x:v>
       </x:c>
     </x:row>
-    <x:row r="18" spans="6:9">
-      <x:c r="F18" t="s">
-        <x:v>42</x:v>
-      </x:c>
-      <x:c r="G18">
+    <x:row r="18" spans="3:4">
+      <x:c r="C18" s="1">
         <x:v>1279</x:v>
       </x:c>
-      <x:c r="H18" t="s">
-        <x:v>31</x:v>
-      </x:c>
-      <x:c r="I18">
+      <x:c r="D18" s="1">
         <x:v>1249</x:v>
       </x:c>
     </x:row>
-    <x:row r="19" spans="6:9">
-      <x:c r="F19" t="s">
-        <x:v>43</x:v>
-      </x:c>
-      <x:c r="G19">
+    <x:row r="19" spans="3:4">
+      <x:c r="C19" s="1">
         <x:v>1282</x:v>
       </x:c>
-      <x:c r="H19" t="s">
-        <x:v>25</x:v>
-      </x:c>
-      <x:c r="I19">
+      <x:c r="D19" s="1">
         <x:v>1252</x:v>
       </x:c>
     </x:row>
-    <x:row r="20" spans="8:9">
-      <x:c r="H20" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="I20">
+    <x:row r="20" spans="4:4">
+      <x:c r="D20" s="1">
         <x:v>1255</x:v>
       </x:c>
     </x:row>
-    <x:row r="21" spans="8:9">
-      <x:c r="H21" t="s">
-        <x:v>44</x:v>
-      </x:c>
-      <x:c r="I21">
+    <x:row r="21" spans="4:4">
+      <x:c r="D21" s="1">
         <x:v>1258</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
-  <x:pageMargins left="0.74805557727813721" right="0.74805557727813721" top="0.98430556058883667" bottom="0.98430556058883667" header="0.51180553436279297" footer="0.51180553436279297"/>
+  <x:pageMargins left="0.74805557727813721" right="0.74805557727813721" top="0.98430556058883667" bottom="0.98430556058883667" header="0.51166665554046631" footer="0.51166665554046631"/>
   <x:pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="0" fitToHeight="0" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" useFirstPageNumber="0" horizontalDpi="600" verticalDpi="600" copies="1"/>
 </x:worksheet>
 </file>
</xml_diff>